<commit_message>
rho -> 1-rho adjustment
</commit_message>
<xml_diff>
--- a/data/Loop on term and rho.xlsx
+++ b/data/Loop on term and rho.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\ISA-Research-Paper\ISA repriced with fixed income\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh4\PycharmProjects\Tracer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19412AA7-3F18-46F4-B5DC-18B6877273B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF960AA4-BDEA-4EC9-A0F4-16C47822230C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10980" yWindow="2985" windowWidth="38865" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -47,7 +48,7 @@
     <t>ISA %</t>
   </si>
   <si>
-    <t>1-rho</t>
+    <t>rho</t>
   </si>
 </sst>
 </file>
@@ -433,7 +434,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -668,7 +669,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D15">
     <sortCondition ref="B2:B15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>